<commit_message>
update jobs & about
</commit_message>
<xml_diff>
--- a/about/Leadership 2023-24.xlsx
+++ b/about/Leadership 2023-24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emma/docs/apls-org/about/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782A819F-2550-8240-90C4-0ECAE687A79C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008526E6-42D5-B142-8CBB-045EE752B450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="13900" windowWidth="21660" windowHeight="13420" firstSheet="18" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="7800" windowWidth="17240" windowHeight="13420" firstSheet="18" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EC" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="429">
   <si>
     <t>Position</t>
   </si>
@@ -1166,24 +1166,9 @@
     <t>2023–2026</t>
   </si>
   <si>
-    <t>Caroline Erentzen</t>
-  </si>
-  <si>
-    <t>erentzen@torontomu.ca</t>
-  </si>
-  <si>
-    <t>Tarika Daftary-Kapur</t>
-  </si>
-  <si>
-    <t>daftarykaput@montclair.edu</t>
-  </si>
-  <si>
     <t>Cassidy Haigh</t>
   </si>
   <si>
-    <t>cassidyhaigh@ufl.edu</t>
-  </si>
-  <si>
     <t>Lauren Kois</t>
   </si>
   <si>
@@ -1338,6 +1323,15 @@
   </si>
   <si>
     <t>Kytazi19@gmail.com</t>
+  </si>
+  <si>
+    <t>Douglas Lewis</t>
+  </si>
+  <si>
+    <t>Will (Minqui) Pan</t>
+  </si>
+  <si>
+    <t>Marco Chavez</t>
   </si>
 </sst>
 </file>
@@ -3722,11 +3716,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2:C2"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3750,27 +3744,27 @@
         <v>68</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>367</v>
+        <v>140</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>80</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>423</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>140</v>
+        <v>367</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>137</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3780,9 +3774,7 @@
       <c r="B4" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>371</v>
-      </c>
+      <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
         <v>372</v>
       </c>
@@ -3794,9 +3786,7 @@
       <c r="B5" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>112</v>
-      </c>
+      <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
         <v>83</v>
       </c>
@@ -3806,11 +3796,9 @@
         <v>72</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>374</v>
-      </c>
+        <v>426</v>
+      </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
         <v>83</v>
       </c>
@@ -3820,27 +3808,33 @@
         <v>72</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>376</v>
-      </c>
+        <v>373</v>
+      </c>
+      <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>210</v>
+        <v>72</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>378</v>
+        <v>427</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>137</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3884,10 +3878,10 @@
         <v>68</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>83</v>
@@ -3898,10 +3892,10 @@
         <v>72</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>71</v>
@@ -3926,10 +3920,10 @@
         <v>72</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>80</v>
@@ -3940,10 +3934,10 @@
         <v>72</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>83</v>
@@ -3990,7 +3984,7 @@
         <v>81</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>75</v>
@@ -4001,10 +3995,10 @@
         <v>72</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>75</v>
@@ -4015,10 +4009,10 @@
         <v>72</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>83</v>
@@ -4029,10 +4023,10 @@
         <v>72</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>83</v>
@@ -4043,10 +4037,10 @@
         <v>210</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>83</v>
@@ -4087,13 +4081,13 @@
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>75</v>
@@ -4101,13 +4095,13 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>83</v>
@@ -4115,7 +4109,7 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>370</v>
@@ -4129,13 +4123,13 @@
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>80</v>
@@ -4143,13 +4137,13 @@
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>83</v>
@@ -4167,7 +4161,7 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
@@ -4207,13 +4201,13 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -4221,7 +4215,7 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>365</v>
@@ -4235,13 +4229,13 @@
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
@@ -4252,10 +4246,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
@@ -4263,13 +4257,13 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>8</v>
@@ -4277,13 +4271,13 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>8</v>
@@ -4291,13 +4285,13 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
@@ -4305,13 +4299,13 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>8</v>
@@ -4319,13 +4313,13 @@
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>8</v>

</xml_diff>